<commit_message>
Pushing code and will use the latest code with Jenkins
</commit_message>
<xml_diff>
--- a/Framework_1/TestData/TestData_1.xlsx
+++ b/Framework_1/TestData/TestData_1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F34F72E-B175-4C9E-B971-9F829433D9CC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A528FE8F-FEB8-49DF-B064-38D643204241}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,10 +26,10 @@
     <t>gaurav.0kr@outlook.com</t>
   </si>
   <si>
-    <t>https://ui.freecrm.com/</t>
+    <t>https://classic.crmpro.com/</t>
   </si>
   <si>
-    <t>Gaurav1234</t>
+    <t>Gaurav123</t>
   </si>
 </sst>
 </file>
@@ -361,7 +361,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -391,7 +391,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>